<commit_message>
Generated a Few Forecast
None of the Forecasts are saved in the database
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/Forecast Results 3M-JAN17.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/Forecast Results 3M-JAN17.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RCK" sheetId="1" r:id="rId1"/>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,18 +535,6 @@
       <c r="D3">
         <v>6794</v>
       </c>
-      <c r="G3" t="str">
-        <f>_xlfn.CONCAT(G2)</f>
-        <v>3075.924102</v>
-      </c>
-      <c r="H3">
-        <f>H2</f>
-        <v>6768.2310254999993</v>
-      </c>
-      <c r="I3">
-        <f>I2</f>
-        <v>20345.919977499998</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -561,10 +549,6 @@
       </c>
       <c r="D4">
         <v>17331</v>
-      </c>
-      <c r="G4" t="str">
-        <f>_xlfn.CONCAT(G3)</f>
-        <v>3075.924102</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1512,7 +1496,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,7 +2544,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3608,7 +3592,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4655,8 +4639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5704,7 +5688,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6752,7 +6736,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7800,7 +7784,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8848,7 +8832,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9896,7 +9880,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10944,7 +10928,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11992,7 +11976,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13040,7 +13024,7 @@
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>